<commit_message>
save report to database
</commit_message>
<xml_diff>
--- a/fact.xlsx
+++ b/fact.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,25 +424,30 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>20180152016</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>大学计算机基础与计算思维</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>必修</t>
-        </is>
-      </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>3.0</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>84</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>2018-2019学年 第1学期</t>
         </is>
@@ -451,25 +456,30 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>20180152016</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>大学生心理健康教育</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>必修</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>2.0</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>96</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>2018-2019学年 第1学期</t>
         </is>
@@ -478,25 +488,30 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>20180152016</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>大学生职业生涯规划</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>必修</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>87</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>2018-2019学年 第1学期</t>
         </is>
@@ -505,25 +520,30 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>高等代数与几何(1)</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>思想道德修养与法律基础</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>2018-2019学年 第1学期</t>
         </is>
@@ -532,25 +552,30 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>军事理论及训练</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>体育(1)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>2018-2019学年 第1学期</t>
         </is>
@@ -559,25 +584,30 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>林学概论</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>英语(1)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>2018-2019学年 第1学期</t>
         </is>
@@ -586,619 +616,734 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>数学分析(1)</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>高等代数与几何(2)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2018-2019学年 第1学期</t>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2018-2019学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>思想道德修养与法律基础</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>体育(2)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>90</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2018-2019学年 第1学期</t>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2018-2019学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>体育(1)</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>英语(2)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2018-2019学年 第1学期</t>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2018-2019学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>英语(1)</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>中国近现代史纲要</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2018-2019学年 第1学期</t>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2018-2019学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>20180152016</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>C语言程序设计</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>必修</t>
-        </is>
-      </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>4.0</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>95</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>2018-2019学年 第2学期</t>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>20180152016</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>C语言程序设计实习</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>必修</t>
-        </is>
-      </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>99</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2018-2019学年 第2学期</t>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>大学生创新创业基础</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>Linux应用</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>2.0</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>83</t>
-        </is>
-      </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2018-2019学年 第2学期</t>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>高等代数与几何(2)</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>电路与模拟电子技术</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2018-2019学年 第2学期</t>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>数学分析(2)</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>高等数学A(1)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2018-2019学年 第2学期</t>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>体育(2)</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>计算机科学与技术导论</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
-      </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2018-2019学年 第2学期</t>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>英语(2)</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>计算机网络</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2018-2019学年 第2学期</t>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>中国近现代史纲要</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>计算机网络实习</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2018-2019学年 第2学期</t>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Java程序设计</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>军事技能</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Linux应用</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>军事理论</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>UI设计</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>数据科学导论</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>UI设计实习</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>Python程序设计实习</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>76</t>
-        </is>
-      </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>大学物理II</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>大学生创新创业基础</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
           <t>83</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>2021-2022学年 第1学期</t>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>电路与模拟电子技术</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>大学物理</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>概率论与数理统计B</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>高等数学A(2)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>计算机科学与技术导论</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>林学概论</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>84</t>
-        </is>
-      </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>计算机网络</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>数据库原理与应用</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>计算机网络实习</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>线性代数A</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0.5</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2020-2021学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>离散数学</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>Java程序设计</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
         <is>
           <t>2021-2022学年 第1学期</t>
         </is>
@@ -1207,25 +1352,30 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>马克思主义基本原理概论</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>UI设计</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
         <is>
           <t>2021-2022学年 第1学期</t>
         </is>
@@ -1234,25 +1384,30 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>数据库原理及应用</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>UI设计实习</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
         <is>
           <t>2021-2022学年 第1学期</t>
         </is>
@@ -1261,25 +1416,30 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>数字逻辑</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>概率论与数理统计B</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>92</t>
-        </is>
-      </c>
       <c r="E32" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
         <is>
           <t>2021-2022学年 第1学期</t>
         </is>
@@ -1288,25 +1448,30 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>体育(3)</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>离散数学</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
         <is>
           <t>2021-2022学年 第1学期</t>
         </is>
@@ -1315,25 +1480,30 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>形势与政策(3)</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>马克思主义基本原理概论</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
         <is>
           <t>2021-2022学年 第1学期</t>
         </is>
@@ -1342,25 +1512,30 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>英语(3)</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>数字逻辑</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
         <is>
           <t>2021-2022学年 第1学期</t>
         </is>
@@ -1369,106 +1544,126 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Python程序设计</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>体育(3)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2021-2022学年 第2学期</t>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2021-2022学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Web程序设计</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>形势与政策(3)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>0.25</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2021-2022学年 第2学期</t>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2021-2022学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Web程序设计实习</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>英语(3)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2021-2022学年 第2学期</t>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2021-2022学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>计算机图形学</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>Python程序设计</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
         <is>
           <t>2021-2022学年 第2学期</t>
         </is>
@@ -1477,25 +1672,30 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>计算机组成原理</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>Web程序设计</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
         <is>
           <t>2021-2022学年 第2学期</t>
         </is>
@@ -1504,25 +1704,30 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>毛泽东思想和中国特色社会主义理论体系概论</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>Web程序设计实习</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
         <is>
           <t>2021-2022学年 第2学期</t>
         </is>
@@ -1531,25 +1736,30 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>数据结构</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>计算机图形学</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>89</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
         <is>
           <t>2021-2022学年 第2学期</t>
         </is>
@@ -1558,25 +1768,30 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>数据结构实习</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>计算机组成原理</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
         <is>
           <t>2021-2022学年 第2学期</t>
         </is>
@@ -1585,25 +1800,30 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>体育(4)</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>毛泽东思想和中国特色社会主义理论体系概论</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
         <is>
           <t>2021-2022学年 第2学期</t>
         </is>
@@ -1612,25 +1832,30 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>无人机技术与应用</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>公修</t>
+          <t>数据结构</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>82</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
         <is>
           <t>2021-2022学年 第2学期</t>
         </is>
@@ -1639,25 +1864,30 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>形势与政策(4)</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>数据结构实习</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
         <is>
           <t>2021-2022学年 第2学期</t>
         </is>
@@ -1666,25 +1896,30 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>英语(4)</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>体育(4)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
         <is>
           <t>2021-2022学年 第2学期</t>
         </is>
@@ -1693,106 +1928,126 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>操作系统原理</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>无人机技术与应用</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>公修</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2022-2023学年 第1学期</t>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>2021-2022学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>考研英语技巧与实训</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>公修</t>
+          <t>形势与政策(4)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>0.25</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2022-2023学年 第1学期</t>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>2021-2022学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>面向对象程序设计(Python)实习</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>英语(4)</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2022-2023学年 第1学期</t>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>2021-2022学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>数据仓库与数据挖掘</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>选修</t>
+          <t>操作系统原理</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
         <is>
           <t>2022-2023学年 第1学期</t>
         </is>
@@ -1801,25 +2056,30 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>形势与政策(5)</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>考研英语技巧与实训</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>公修</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
         <is>
           <t>2022-2023学年 第1学期</t>
         </is>
@@ -1828,25 +2088,30 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>遥感原理与遥感图像处理</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
+          <t>数据仓库与数据挖掘</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
           <t>选修</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
         <is>
           <t>2022-2023学年 第1学期</t>
         </is>
@@ -1855,25 +2120,30 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>移动应用开发</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>形势与政策(5)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>0.25</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
         <is>
           <t>2022-2023学年 第1学期</t>
         </is>
@@ -1882,25 +2152,30 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>综合实习一</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>遥感原理与遥感图像处理</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>选修</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
         <is>
           <t>2022-2023学年 第1学期</t>
         </is>
@@ -1909,79 +2184,94 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>编译技术</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>移动应用开发</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2022-2023学年 第2学期</t>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>2022-2023学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>大数据平台技术</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>选修</t>
+          <t>综合实习一</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2022-2023学年 第2学期</t>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>2022-2023学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>就业指导</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>编译技术</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
         <is>
           <t>2022-2023学年 第2学期</t>
         </is>
@@ -1990,25 +2280,30 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>软件工程</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>大数据平台技术</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
+          <t>选修</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
           <t>3.0</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>85</t>
-        </is>
-      </c>
       <c r="E59" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
         <is>
           <t>2022-2023学年 第2学期</t>
         </is>
@@ -2017,25 +2312,30 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>算法设计与分析</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>就业指导</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
         <is>
           <t>2022-2023学年 第2学期</t>
         </is>
@@ -2044,25 +2344,30 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>形势与政策(6)</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>软件工程</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
           <t>85</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
+      <c r="F61" t="inlineStr">
         <is>
           <t>2022-2023学年 第2学期</t>
         </is>
@@ -2071,25 +2376,30 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>中国古典小说巅峰-四大名著鉴赏</t>
+          <t>20180152016</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>公修</t>
+          <t>算法设计与分析</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
         <is>
           <t>2022-2023学年 第2学期</t>
         </is>
@@ -2098,27 +2408,224 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
+          <t>20180152016</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>形势与政策(6)</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>2022-2023学年 第2学期</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>20180152016</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>中国古典小说巅峰-四大名著鉴赏</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>公修</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>2022-2023学年 第2学期</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>20180152016</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
           <t>综合实习二</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>必修</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
         <is>
           <t>3.0</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
+      <c r="E65" t="inlineStr">
         <is>
           <t>88</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
+      <c r="F65" t="inlineStr">
         <is>
           <t>2022-2023学年 第2学期</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>20180152016</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>计算机系统结构</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>2023-2024学年 第1学期</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>20180152016</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>形势与政策(7)</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>2023-2024学年 第1学期</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>20180152016</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>行为生活方式与健康</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>公修</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>2023-2024学年 第1学期</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>20180152016</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>林学概论实习</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>2023-2024学年 第2学期</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
half work to control the rule
</commit_message>
<xml_diff>
--- a/fact.xlsx
+++ b/fact.xlsx
@@ -424,7 +424,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,7 +488,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -520,7 +520,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -552,7 +552,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -584,7 +584,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -616,7 +616,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -648,7 +648,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -680,7 +680,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -712,7 +712,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -744,7 +744,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -776,7 +776,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -840,7 +840,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -872,7 +872,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -904,7 +904,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -936,7 +936,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1000,7 +1000,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1032,7 +1032,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1064,7 +1064,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1096,7 +1096,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1128,7 +1128,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1160,7 +1160,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1192,7 +1192,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1224,7 +1224,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1256,7 +1256,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1288,7 +1288,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1320,7 +1320,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1352,7 +1352,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1384,7 +1384,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1416,7 +1416,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1480,7 +1480,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1512,7 +1512,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1544,7 +1544,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1576,7 +1576,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1608,7 +1608,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1640,7 +1640,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1672,7 +1672,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1704,7 +1704,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1736,7 +1736,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1768,7 +1768,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1800,7 +1800,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1832,7 +1832,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1864,7 +1864,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1896,7 +1896,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1960,7 +1960,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1992,7 +1992,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2024,7 +2024,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2056,7 +2056,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2088,7 +2088,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2120,7 +2120,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2152,7 +2152,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2184,7 +2184,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2216,7 +2216,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2248,7 +2248,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2280,7 +2280,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2312,7 +2312,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2344,7 +2344,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2376,7 +2376,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>20210352026</t>
+          <t>20180300052016</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">

</xml_diff>

<commit_message>
modify some code about the database
</commit_message>
<xml_diff>
--- a/fact.xlsx
+++ b/fact.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,7 +424,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,7 +488,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -520,12 +520,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>高等代数与几何(1)</t>
+          <t>思想道德修养与法律基础</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -535,12 +535,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>90</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -552,12 +552,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>军事理论及训练</t>
+          <t>体育(1)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -567,12 +567,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>81</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -584,12 +584,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>林学概论</t>
+          <t>英语(1)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -599,12 +599,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -616,12 +616,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>数学分析(1)</t>
+          <t>高等代数与几何(2)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -631,29 +631,29 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>97</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2018-2019学年 第1学期</t>
+          <t>2018-2019学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>思想道德修养与法律基础</t>
+          <t>体育(2)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -663,7 +663,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -673,19 +673,19 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2018-2019学年 第1学期</t>
+          <t>2018-2019学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>体育(1)</t>
+          <t>英语(2)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -695,29 +695,29 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2018-2019学年 第1学期</t>
+          <t>2018-2019学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>英语(1)</t>
+          <t>中国近现代史纲要</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -727,24 +727,24 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2018-2019学年 第1学期</t>
+          <t>2018-2019学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -769,14 +769,14 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2018-2019学年 第2学期</t>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -791,7 +791,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -801,19 +801,19 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2018-2019学年 第2学期</t>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>大学生创新创业基础</t>
+          <t>Linux应用</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -828,24 +828,24 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>92</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2018-2019学年 第2学期</t>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>高等代数与几何(2)</t>
+          <t>电路与模拟电子技术</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -855,29 +855,29 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>92</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2018-2019学年 第2学期</t>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>数学分析(2)</t>
+          <t>高等数学A(1)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -887,29 +887,29 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>98</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2018-2019学年 第2学期</t>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>体育(2)</t>
+          <t>计算机科学与技术导论</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -924,24 +924,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>84</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2018-2019学年 第2学期</t>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>英语(2)</t>
+          <t>计算机网络</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -951,29 +951,29 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>92</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2018-2019学年 第2学期</t>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>中国近现代史纲要</t>
+          <t>计算机网络实习</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -983,29 +983,29 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>96</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2018-2019学年 第2学期</t>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Java程序设计</t>
+          <t>军事技能</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1015,29 +1015,29 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>79</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Linux应用</t>
+          <t>军事理论</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1047,29 +1047,29 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>79</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>UI设计</t>
+          <t>数据科学导论</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1079,29 +1079,29 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>78</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>2020-2021学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>UI设计实习</t>
+          <t>Python程序设计实习</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1116,24 +1116,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>76</t>
+          <t>81</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>2020-2021学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>大学物理II</t>
+          <t>大学生创新创业基础</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1153,19 +1153,19 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>2020-2021学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>电路与模拟电子技术</t>
+          <t>大学物理</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1175,29 +1175,29 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>2020-2021学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>概率论与数理统计B</t>
+          <t>高等数学A(2)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1207,29 +1207,29 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>96</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>2020-2021学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>计算机科学与技术导论</t>
+          <t>林学概论</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1244,24 +1244,24 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>85</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>2020-2021学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>计算机网络</t>
+          <t>数据库原理与应用</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1271,29 +1271,29 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>81</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>2020-2021学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>计算机网络实习</t>
+          <t>线性代数A</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1303,29 +1303,29 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>98</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2021-2022学年 第1学期</t>
+          <t>2020-2021学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>离散数学</t>
+          <t>Java程序设计</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1335,12 +1335,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>92</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1352,12 +1352,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>马克思主义基本原理概论</t>
+          <t>UI设计</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1367,12 +1367,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>91</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1384,12 +1384,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>数据库原理及应用</t>
+          <t>UI设计实习</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1399,12 +1399,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>76</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1416,12 +1416,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>数字逻辑</t>
+          <t>概率论与数理统计B</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1448,12 +1448,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>体育(3)</t>
+          <t>离散数学</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1463,12 +1463,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>97</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1480,12 +1480,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>形势与政策(3)</t>
+          <t>马克思主义基本原理概论</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1495,12 +1495,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>92</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1512,12 +1512,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>英语(3)</t>
+          <t>数字逻辑</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1527,12 +1527,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>92</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1544,12 +1544,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Python程序设计</t>
+          <t>体育(3)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1559,29 +1559,29 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2021-2022学年 第2学期</t>
+          <t>2021-2022学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Web程序设计</t>
+          <t>形势与政策(3)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1591,29 +1591,29 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0.25</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>90</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2021-2022学年 第2学期</t>
+          <t>2021-2022学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Web程序设计实习</t>
+          <t>英语(3)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1623,29 +1623,29 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>86</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2021-2022学年 第2学期</t>
+          <t>2021-2022学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>计算机图形学</t>
+          <t>Python程序设计</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1655,12 +1655,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>72</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1672,12 +1672,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>计算机组成原理</t>
+          <t>Web程序设计</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1687,12 +1687,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -1704,12 +1704,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>毛泽东思想和中国特色社会主义理论体系概论</t>
+          <t>Web程序设计实习</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1719,12 +1719,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1736,12 +1736,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>数据结构</t>
+          <t>计算机图形学</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1751,12 +1751,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>89</t>
+          <t>91</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1768,12 +1768,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>数据结构实习</t>
+          <t>计算机组成原理</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1783,12 +1783,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>90</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1800,12 +1800,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>体育(4)</t>
+          <t>毛泽东思想和中国特色社会主义理论体系概论</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1815,12 +1815,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>85</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1832,27 +1832,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>无人机技术与应用</t>
+          <t>数据结构</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>公修</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>82</t>
+          <t>89</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -1864,12 +1864,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>形势与政策(4)</t>
+          <t>数据结构实习</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1879,12 +1879,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>94</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -1896,12 +1896,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>英语(4)</t>
+          <t>体育(4)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1911,12 +1911,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>90</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -1928,76 +1928,76 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>操作系统原理</t>
+          <t>无人机技术与应用</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>公修</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>82</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2022-2023学年 第1学期</t>
+          <t>2021-2022学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>考研英语技巧与实训</t>
+          <t>形势与政策(4)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>公修</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>0.25</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>85</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2022-2023学年 第1学期</t>
+          <t>2021-2022学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>面向对象程序设计(Python)实习</t>
+          <t>英语(4)</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2007,44 +2007,44 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>78</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2022-2023学年 第1学期</t>
+          <t>2021-2022学年 第2学期</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>数据仓库与数据挖掘</t>
+          <t>操作系统原理</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>选修</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>98</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2056,27 +2056,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>形势与政策(5)</t>
+          <t>考研英语技巧与实训</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>公修</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>84</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2088,12 +2088,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>遥感原理与遥感图像处理</t>
+          <t>数据仓库与数据挖掘</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2103,12 +2103,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>80</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -2120,12 +2120,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>移动应用开发</t>
+          <t>形势与政策(5)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2135,12 +2135,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>0.25</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>85</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -2152,27 +2152,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>综合实习一</t>
+          <t>遥感原理与遥感图像处理</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>选修</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>92</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2184,12 +2184,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>编译技术</t>
+          <t>移动应用开发</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2199,61 +2199,61 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>98</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2022-2023学年 第2学期</t>
+          <t>2022-2023学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>大数据平台技术</t>
+          <t>综合实习一</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>选修</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2022-2023学年 第2学期</t>
+          <t>2022-2023学年 第1学期</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>就业指导</t>
+          <t>编译技术</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2263,12 +2263,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>70</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -2280,17 +2280,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>软件工程</t>
+          <t>大数据平台技术</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>必修</t>
+          <t>选修</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2300,7 +2300,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>96</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -2312,12 +2312,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>算法设计与分析</t>
+          <t>就业指导</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2327,12 +2327,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>90</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2344,12 +2344,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>形势与政策(6)</t>
+          <t>软件工程</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2376,27 +2376,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>中国古典小说巅峰-四大名著鉴赏</t>
+          <t>算法设计与分析</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>公修</t>
+          <t>必修</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>94</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2408,32 +2408,224 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>20180300052016</t>
+          <t>20180152099</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
+          <t>形势与政策(6)</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>2022-2023学年 第2学期</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>20180152099</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>中国古典小说巅峰-四大名著鉴赏</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>公修</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>2022-2023学年 第2学期</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>20180152099</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
           <t>综合实习二</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>必修</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
         <is>
           <t>3.0</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
+      <c r="E65" t="inlineStr">
         <is>
           <t>88</t>
         </is>
       </c>
-      <c r="F63" t="inlineStr">
+      <c r="F65" t="inlineStr">
         <is>
           <t>2022-2023学年 第2学期</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>20180152099</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>计算机系统结构</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>2023-2024学年 第1学期</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>20180152099</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>形势与政策(7)</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>2023-2024学年 第1学期</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>20180152099</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>行为生活方式与健康</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>公修</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>2023-2024学年 第1学期</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>20180152099</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>林学概论实习</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>必修</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>2023-2024学年 第2学期</t>
         </is>
       </c>
     </row>

</xml_diff>